<commit_message>
docker - working - fixed typos
</commit_message>
<xml_diff>
--- a/marketplace-service/src/main/resources/products.xlsx
+++ b/marketplace-service/src/main/resources/products.xlsx
@@ -527,7 +527,7 @@
     <col min="5" max="5" style="3" width="22.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -561,7 +561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -595,7 +595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -612,7 +612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -629,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -646,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -663,7 +663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -677,10 +677,10 @@
         <v>2000</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
         <v>109</v>
       </c>
@@ -697,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1">
         <v>110</v>
       </c>
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1">
         <v>111</v>
       </c>

</xml_diff>